<commit_message>
Multiple changes and speed improvements
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="atoms" sheetId="2" r:id="rId1"/>
     <sheet name="amino_acids" sheetId="1" r:id="rId2"/>
     <sheet name="losses" sheetId="3" r:id="rId3"/>
     <sheet name="ion_type_list" sheetId="4" r:id="rId4"/>
+    <sheet name="term" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="131">
   <si>
     <t>FullName</t>
   </si>
@@ -339,18 +340,6 @@
     <t>Electron</t>
   </si>
   <si>
-    <t>AminoAcid</t>
-  </si>
-  <si>
-    <t>Loss</t>
-  </si>
-  <si>
-    <t>Gain</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>H2O</t>
   </si>
   <si>
@@ -403,6 +392,30 @@
   </si>
   <si>
     <t>AverageMass</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>NH2</t>
+  </si>
+  <si>
+    <t>CH3CO</t>
+  </si>
+  <si>
+    <t>NH2CO</t>
+  </si>
+  <si>
+    <t>C6H4CO</t>
+  </si>
+  <si>
+    <t>terminus</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>term</t>
   </si>
 </sst>
 </file>
@@ -1211,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,10 +1238,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,19 +1447,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="C1" sqref="C1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="16" max="16" width="20.140625" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1493,13 +1507,16 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="Q1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="R1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1546,15 +1563,16 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <f>E2*atoms!C$2+F2*atoms!C$3+G2*atoms!C$4+H2*atoms!C$5+I2*atoms!C$6+J2*atoms!C$7+K2*atoms!C$8+L2*atoms!C$9+M2*atoms!C$10+N2*atoms!C$11+O2*atoms!C$12</f>
-        <v>71.037113779999999</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <f>E2*atoms!D$2+F2*atoms!D$3+G2*atoms!D$4+H2*atoms!D$5+I2*atoms!D$6+J2*atoms!D$7+K2*atoms!D$8+L2*atoms!D$9+M2*atoms!D$10+N2*atoms!D$11+O2*atoms!D$12</f>
-        <v>71.077930000000009</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1601,15 +1619,16 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <f>E3*atoms!C$2+F3*atoms!C$3+G3*atoms!C$4+H3*atoms!C$5+I3*atoms!C$6+J3*atoms!C$7+K3*atoms!C$8+L3*atoms!C$9+M3*atoms!C$10+N3*atoms!C$11+O3*atoms!C$12</f>
-        <v>156.10111100399999</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <f>E3*atoms!D$2+F3*atoms!D$3+G3*atoms!D$4+H3*atoms!D$5+I3*atoms!D$6+J3*atoms!D$7+K3*atoms!D$8+L3*atoms!D$9+M3*atoms!D$10+N3*atoms!D$11+O3*atoms!D$12</f>
-        <v>156.18612000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1656,15 +1675,16 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <f>E4*atoms!C$2+F4*atoms!C$3+G4*atoms!C$4+H4*atoms!C$5+I4*atoms!C$6+J4*atoms!C$7+K4*atoms!C$8+L4*atoms!C$9+M4*atoms!C$10+N4*atoms!C$11+O4*atoms!C$12</f>
-        <v>126.042927432</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <f>E4*atoms!D$2+F4*atoms!D$3+G4*atoms!D$4+H4*atoms!D$5+I4*atoms!D$6+J4*atoms!D$7+K4*atoms!D$8+L4*atoms!D$9+M4*atoms!D$10+N4*atoms!D$11+O4*atoms!D$12</f>
-        <v>126.11336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1711,15 +1731,16 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <f>E5*atoms!C$2+F5*atoms!C$3+G5*atoms!C$4+H5*atoms!C$5+I5*atoms!C$6+J5*atoms!C$7+K5*atoms!C$8+L5*atoms!C$9+M5*atoms!C$10+N5*atoms!C$11+O5*atoms!C$12</f>
-        <v>127.02694301999999</v>
+        <v>0</v>
       </c>
       <c r="Q5">
-        <f>E5*atoms!D$2+F5*atoms!D$3+G5*atoms!D$4+H5*atoms!D$5+I5*atoms!D$6+J5*atoms!D$7+K5*atoms!D$8+L5*atoms!D$9+M5*atoms!D$10+N5*atoms!D$11+O5*atoms!D$12</f>
-        <v>127.09792999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1766,15 +1787,16 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <f>E6*atoms!C$2+F6*atoms!C$3+G6*atoms!C$4+H6*atoms!C$5+I6*atoms!C$6+J6*atoms!C$7+K6*atoms!C$8+L6*atoms!C$9+M6*atoms!C$10+N6*atoms!C$11+O6*atoms!C$12</f>
-        <v>103.00918494999999</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <f>E6*atoms!D$2+F6*atoms!D$3+G6*atoms!D$4+H6*atoms!D$5+I6*atoms!D$6+J6*atoms!D$7+K6*atoms!D$8+L6*atoms!D$9+M6*atoms!D$10+N6*atoms!D$11+O6*atoms!D$12</f>
-        <v>103.14543</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1821,15 +1843,16 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <f>E7*atoms!C$2+F7*atoms!C$3+G7*atoms!C$4+H7*atoms!C$5+I7*atoms!C$6+J7*atoms!C$7+K7*atoms!C$8+L7*atoms!C$9+M7*atoms!C$10+N7*atoms!C$11+O7*atoms!C$12</f>
-        <v>129.04259308399998</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <f>E7*atoms!D$2+F7*atoms!D$3+G7*atoms!D$4+H7*atoms!D$5+I7*atoms!D$6+J7*atoms!D$7+K7*atoms!D$8+L7*atoms!D$9+M7*atoms!D$10+N7*atoms!D$11+O7*atoms!D$12</f>
-        <v>129.11387999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1876,15 +1899,16 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <f>E8*atoms!C$2+F8*atoms!C$3+G8*atoms!C$4+H8*atoms!C$5+I8*atoms!C$6+J8*atoms!C$7+K8*atoms!C$8+L8*atoms!C$9+M8*atoms!C$10+N8*atoms!C$11+O8*atoms!C$12</f>
-        <v>128.058577496</v>
+        <v>0</v>
       </c>
       <c r="Q8">
-        <f>E8*atoms!D$2+F8*atoms!D$3+G8*atoms!D$4+H8*atoms!D$5+I8*atoms!D$6+J8*atoms!D$7+K8*atoms!D$8+L8*atoms!D$9+M8*atoms!D$10+N8*atoms!D$11+O8*atoms!D$12</f>
-        <v>128.12931</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1931,15 +1955,16 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <f>E9*atoms!C$2+F9*atoms!C$3+G9*atoms!C$4+H9*atoms!C$5+I9*atoms!C$6+J9*atoms!C$7+K9*atoms!C$8+L9*atoms!C$9+M9*atoms!C$10+N9*atoms!C$11+O9*atoms!C$12</f>
-        <v>57.021463716</v>
+        <v>0</v>
       </c>
       <c r="Q9">
-        <f>E9*atoms!D$2+F9*atoms!D$3+G9*atoms!D$4+H9*atoms!D$5+I9*atoms!D$6+J9*atoms!D$7+K9*atoms!D$8+L9*atoms!D$9+M9*atoms!D$10+N9*atoms!D$11+O9*atoms!D$12</f>
-        <v>57.051380000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1986,15 +2011,16 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <f>E10*atoms!C$2+F10*atoms!C$3+G10*atoms!C$4+H10*atoms!C$5+I10*atoms!C$6+J10*atoms!C$7+K10*atoms!C$8+L10*atoms!C$9+M10*atoms!C$10+N10*atoms!C$11+O10*atoms!C$12</f>
-        <v>137.05891184399999</v>
+        <v>0</v>
       </c>
       <c r="Q10">
-        <f>E10*atoms!D$2+F10*atoms!D$3+G10*atoms!D$4+H10*atoms!D$5+I10*atoms!D$6+J10*atoms!D$7+K10*atoms!D$8+L10*atoms!D$9+M10*atoms!D$10+N10*atoms!D$11+O10*atoms!D$12</f>
-        <v>137.13939000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2041,15 +2067,16 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <f>E11*atoms!C$2+F11*atoms!C$3+G11*atoms!C$4+H11*atoms!C$5+I11*atoms!C$6+J11*atoms!C$7+K11*atoms!C$8+L11*atoms!C$9+M11*atoms!C$10+N11*atoms!C$11+O11*atoms!C$12</f>
-        <v>113.084063972</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <f>E11*atoms!D$2+F11*atoms!D$3+G11*atoms!D$4+H11*atoms!D$5+I11*atoms!D$6+J11*atoms!D$7+K11*atoms!D$8+L11*atoms!D$9+M11*atoms!D$10+N11*atoms!D$11+O11*atoms!D$12</f>
-        <v>113.15758000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2096,15 +2123,16 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <f>E12*atoms!C$2+F12*atoms!C$3+G12*atoms!C$4+H12*atoms!C$5+I12*atoms!C$6+J12*atoms!C$7+K12*atoms!C$8+L12*atoms!C$9+M12*atoms!C$10+N12*atoms!C$11+O12*atoms!C$12</f>
-        <v>113.084063972</v>
+        <v>0</v>
       </c>
       <c r="Q12">
-        <f>E12*atoms!D$2+F12*atoms!D$3+G12*atoms!D$4+H12*atoms!D$5+I12*atoms!D$6+J12*atoms!D$7+K12*atoms!D$8+L12*atoms!D$9+M12*atoms!D$10+N12*atoms!D$11+O12*atoms!D$12</f>
-        <v>113.15758000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2151,15 +2179,16 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <f>E13*atoms!C$2+F13*atoms!C$3+G13*atoms!C$4+H13*atoms!C$5+I13*atoms!C$6+J13*atoms!C$7+K13*atoms!C$8+L13*atoms!C$9+M13*atoms!C$10+N13*atoms!C$11+O13*atoms!C$12</f>
-        <v>128.09496300399999</v>
+        <v>0</v>
       </c>
       <c r="Q13">
-        <f>E13*atoms!D$2+F13*atoms!D$3+G13*atoms!D$4+H13*atoms!D$5+I13*atoms!D$6+J13*atoms!D$7+K13*atoms!D$8+L13*atoms!D$9+M13*atoms!D$10+N13*atoms!D$11+O13*atoms!D$12</f>
-        <v>128.17241000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2206,15 +2235,16 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <f>E14*atoms!C$2+F14*atoms!C$3+G14*atoms!C$4+H14*atoms!C$5+I14*atoms!C$6+J14*atoms!C$7+K14*atoms!C$8+L14*atoms!C$9+M14*atoms!C$10+N14*atoms!C$11+O14*atoms!C$12</f>
-        <v>131.04048507799999</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <f>E14*atoms!D$2+F14*atoms!D$3+G14*atoms!D$4+H14*atoms!D$5+I14*atoms!D$6+J14*atoms!D$7+K14*atoms!D$8+L14*atoms!D$9+M14*atoms!D$10+N14*atoms!D$11+O14*atoms!D$12</f>
-        <v>131.19853000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -2261,15 +2291,16 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <f>E15*atoms!C$2+F15*atoms!C$3+G15*atoms!C$4+H15*atoms!C$5+I15*atoms!C$6+J15*atoms!C$7+K15*atoms!C$8+L15*atoms!C$9+M15*atoms!C$10+N15*atoms!C$11+O15*atoms!C$12</f>
-        <v>147.068413908</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <f>E15*atoms!D$2+F15*atoms!D$3+G15*atoms!D$4+H15*atoms!D$5+I15*atoms!D$6+J15*atoms!D$7+K15*atoms!D$8+L15*atoms!D$9+M15*atoms!D$10+N15*atoms!D$11+O15*atoms!D$12</f>
-        <v>147.17343</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2316,15 +2347,16 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <f>E16*atoms!C$2+F16*atoms!C$3+G16*atoms!C$4+H16*atoms!C$5+I16*atoms!C$6+J16*atoms!C$7+K16*atoms!C$8+L16*atoms!C$9+M16*atoms!C$10+N16*atoms!C$11+O16*atoms!C$12</f>
-        <v>97.052763843999998</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <f>E16*atoms!D$2+F16*atoms!D$3+G16*atoms!D$4+H16*atoms!D$5+I16*atoms!D$6+J16*atoms!D$7+K16*atoms!D$8+L16*atoms!D$9+M16*atoms!D$10+N16*atoms!D$11+O16*atoms!D$12</f>
-        <v>97.115079999999992</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2371,15 +2403,16 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <f>E17*atoms!C$2+F17*atoms!C$3+G17*atoms!C$4+H17*atoms!C$5+I17*atoms!C$6+J17*atoms!C$7+K17*atoms!C$8+L17*atoms!C$9+M17*atoms!C$10+N17*atoms!C$11+O17*atoms!C$12</f>
-        <v>87.032028400000002</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <f>E17*atoms!D$2+F17*atoms!D$3+G17*atoms!D$4+H17*atoms!D$5+I17*atoms!D$6+J17*atoms!D$7+K17*atoms!D$8+L17*atoms!D$9+M17*atoms!D$10+N17*atoms!D$11+O17*atoms!D$12</f>
-        <v>87.077330000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2426,15 +2459,16 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <f>E18*atoms!C$2+F18*atoms!C$3+G18*atoms!C$4+H18*atoms!C$5+I18*atoms!C$6+J18*atoms!C$7+K18*atoms!C$8+L18*atoms!C$9+M18*atoms!C$10+N18*atoms!C$11+O18*atoms!C$12</f>
-        <v>101.047678464</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <f>E18*atoms!D$2+F18*atoms!D$3+G18*atoms!D$4+H18*atoms!D$5+I18*atoms!D$6+J18*atoms!D$7+K18*atoms!D$8+L18*atoms!D$9+M18*atoms!D$10+N18*atoms!D$11+O18*atoms!D$12</f>
-        <v>101.10388</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -2481,15 +2515,16 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <f>E19*atoms!C$2+F19*atoms!C$3+G19*atoms!C$4+H19*atoms!C$5+I19*atoms!C$6+J19*atoms!C$7+K19*atoms!C$8+L19*atoms!C$9+M19*atoms!C$10+N19*atoms!C$11+O19*atoms!C$12</f>
-        <v>186.07931293999999</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <f>E19*atoms!D$2+F19*atoms!D$3+G19*atoms!D$4+H19*atoms!D$5+I19*atoms!D$6+J19*atoms!D$7+K19*atoms!D$8+L19*atoms!D$9+M19*atoms!D$10+N19*atoms!D$11+O19*atoms!D$12</f>
-        <v>186.20946000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -2536,15 +2571,16 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <f>E20*atoms!C$2+F20*atoms!C$3+G20*atoms!C$4+H20*atoms!C$5+I20*atoms!C$6+J20*atoms!C$7+K20*atoms!C$8+L20*atoms!C$9+M20*atoms!C$10+N20*atoms!C$11+O20*atoms!C$12</f>
-        <v>163.063328528</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <f>E20*atoms!D$2+F20*atoms!D$3+G20*atoms!D$4+H20*atoms!D$5+I20*atoms!D$6+J20*atoms!D$7+K20*atoms!D$8+L20*atoms!D$9+M20*atoms!D$10+N20*atoms!D$11+O20*atoms!D$12</f>
-        <v>163.17282999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -2591,12 +2627,13 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <f>E21*atoms!C$2+F21*atoms!C$3+G21*atoms!C$4+H21*atoms!C$5+I21*atoms!C$6+J21*atoms!C$7+K21*atoms!C$8+L21*atoms!C$9+M21*atoms!C$10+N21*atoms!C$11+O21*atoms!C$12</f>
-        <v>99.068413907999997</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <f>E21*atoms!D$2+F21*atoms!D$3+G21*atoms!D$4+H21*atoms!D$5+I21*atoms!D$6+J21*atoms!D$7+K21*atoms!D$8+L21*atoms!D$9+M21*atoms!D$10+N21*atoms!D$11+O21*atoms!D$12</f>
-        <v>99.131029999999996</v>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2607,95 +2644,368 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2705,64 +3015,847 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>-2</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>-1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2788,25 +3881,37 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2826,25 +3931,37 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4">
-        <v>-1</v>
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2864,25 +3981,37 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2902,58 +4031,82 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>-1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -2978,312 +4131,21 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>-1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>-1</v>
-      </c>
-      <c r="D10">
-        <v>-1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>-2</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B12">
-        <v>-1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>-1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>-1</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed d,v,w ion generation
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="atoms" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="161">
   <si>
     <t>FullName</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t>exchangeable_deuteriums</t>
+  </si>
+  <si>
+    <t>partial_sidechain_prime</t>
+  </si>
+  <si>
+    <t>d'</t>
+  </si>
+  <si>
+    <t>w'</t>
   </si>
 </sst>
 </file>
@@ -1606,14 +1615,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="6" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="17" max="17" width="7.7109375" customWidth="1"/>
     <col min="18" max="18" width="6.5703125" customWidth="1"/>
     <col min="19" max="19" width="6.140625" customWidth="1"/>
@@ -3480,14 +3490,14 @@
   <dimension ref="A1:T62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" customWidth="1"/>
     <col min="14" max="14" width="6.5703125" customWidth="1"/>
     <col min="15" max="15" width="6.140625" customWidth="1"/>
@@ -4738,7 +4748,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -5420,7 +5430,7 @@
         <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -5544,7 +5554,7 @@
         <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -7345,10 +7355,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8104,13 +8114,13 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -8119,7 +8129,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -8166,7 +8176,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -8175,10 +8185,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -8228,77 +8238,201 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>-1</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>116</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>1</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed AA mass errors
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="atoms" sheetId="2" r:id="rId1"/>
@@ -466,9 +466,6 @@
     <t>tyr</t>
   </si>
   <si>
-    <t>C9H10O5N</t>
-  </si>
-  <si>
     <t>C3H5ONSe</t>
   </si>
   <si>
@@ -506,6 +503,9 @@
   </si>
   <si>
     <t>sidechain</t>
+  </si>
+  <si>
+    <t>C9H10O5NP</t>
   </si>
 </sst>
 </file>
@@ -1615,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1646,7 @@
         <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1871,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>6</v>
@@ -1945,7 +1945,7 @@
         <v>2</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -2898,7 +2898,7 @@
         <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E18">
         <v>-1</v>
@@ -3046,7 +3046,7 @@
         <v>137</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E20">
         <v>-1</v>
@@ -3120,7 +3120,7 @@
         <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -3342,7 +3342,7 @@
         <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -3366,7 +3366,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -3489,7 +3489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
@@ -3520,7 +3520,7 @@
         <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
         <v>114</v>
@@ -3529,10 +3529,10 @@
         <v>115</v>
       </c>
       <c r="G1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
         <v>159</v>
-      </c>
-      <c r="H1" t="s">
-        <v>160</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3594,7 +3594,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3662,7 +3662,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3730,7 +3730,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3798,7 +3798,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3866,7 +3866,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -3934,7 +3934,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -4002,7 +4002,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -4070,7 +4070,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -4138,7 +4138,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -4206,7 +4206,7 @@
         <v>136</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -4274,7 +4274,7 @@
         <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -4342,7 +4342,7 @@
         <v>137</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -4410,7 +4410,7 @@
         <v>109</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -4478,7 +4478,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -4549,7 +4549,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -4620,7 +4620,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -4691,7 +4691,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -4762,7 +4762,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -4833,7 +4833,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -4904,7 +4904,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -4975,7 +4975,7 @@
         <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -5046,7 +5046,7 @@
         <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -5117,7 +5117,7 @@
         <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -5188,7 +5188,7 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -5259,7 +5259,7 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -5327,7 +5327,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -5398,7 +5398,7 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -5469,7 +5469,7 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -5537,7 +5537,7 @@
         <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -5605,7 +5605,7 @@
         <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -5673,7 +5673,7 @@
         <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -5741,7 +5741,7 @@
         <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -5809,7 +5809,7 @@
         <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -5877,7 +5877,7 @@
         <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -5948,7 +5948,7 @@
         <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -6016,7 +6016,7 @@
         <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -6087,7 +6087,7 @@
         <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -6155,7 +6155,7 @@
         <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -6223,7 +6223,7 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -6288,7 +6288,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -6353,7 +6353,7 @@
         <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -6418,7 +6418,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -6483,7 +6483,7 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -6548,7 +6548,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -6613,7 +6613,7 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -6678,7 +6678,7 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -6743,7 +6743,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -6808,7 +6808,7 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -6873,7 +6873,7 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -6938,7 +6938,7 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -7003,7 +7003,7 @@
         <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -7068,7 +7068,7 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -7133,7 +7133,7 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -7198,7 +7198,7 @@
         <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -7263,7 +7263,7 @@
         <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -7328,7 +7328,7 @@
         <v>137</v>
       </c>
       <c r="B57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -7393,7 +7393,7 @@
         <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -7458,7 +7458,7 @@
         <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -7523,7 +7523,7 @@
         <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -7588,7 +7588,7 @@
         <v>80</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -7653,7 +7653,7 @@
         <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -7718,7 +7718,7 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -7783,7 +7783,7 @@
         <v>34</v>
       </c>
       <c r="B64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -7848,7 +7848,7 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -7913,7 +7913,7 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -7978,7 +7978,7 @@
         <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -8043,7 +8043,7 @@
         <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -8108,7 +8108,7 @@
         <v>38</v>
       </c>
       <c r="B69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -8173,7 +8173,7 @@
         <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -8238,7 +8238,7 @@
         <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -8303,7 +8303,7 @@
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -8368,7 +8368,7 @@
         <v>80</v>
       </c>
       <c r="B73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -8433,7 +8433,7 @@
         <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -9260,7 +9260,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -9446,7 +9446,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Fixed neutral losses issue
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="13650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="atoms" sheetId="2" r:id="rId1"/>
@@ -5384,9 +5384,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X8" sqref="X8"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10620,7 +10620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bugs, separated out M*-sidechain and fragment-sidechain.
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="163">
   <si>
     <t>FullName</t>
   </si>
@@ -6414,9 +6414,6 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>158</v>
-      </c>
       <c r="C15">
         <v>1</v>
       </c>
@@ -6488,9 +6485,6 @@
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
-        <v>158</v>
-      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -6562,9 +6556,6 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>158</v>
-      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -6636,9 +6627,6 @@
       <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
-        <v>158</v>
-      </c>
       <c r="C18">
         <v>1</v>
       </c>
@@ -6710,9 +6698,6 @@
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
-        <v>158</v>
-      </c>
       <c r="C19">
         <v>1</v>
       </c>
@@ -6784,9 +6769,6 @@
       <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
-        <v>158</v>
-      </c>
       <c r="C20">
         <v>1</v>
       </c>
@@ -6858,9 +6840,6 @@
       <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21" t="s">
-        <v>158</v>
-      </c>
       <c r="D21">
         <v>1</v>
       </c>
@@ -6932,9 +6911,6 @@
       <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="B22" t="s">
-        <v>158</v>
-      </c>
       <c r="C22">
         <v>1</v>
       </c>
@@ -7006,9 +6982,6 @@
       <c r="A23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
-        <v>158</v>
-      </c>
       <c r="C23">
         <v>1</v>
       </c>
@@ -7080,9 +7053,6 @@
       <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
-        <v>158</v>
-      </c>
       <c r="C24">
         <v>1</v>
       </c>
@@ -7154,9 +7124,6 @@
       <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
-        <v>158</v>
-      </c>
       <c r="C25">
         <v>1</v>
       </c>
@@ -7228,9 +7195,6 @@
       <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="B26" t="s">
-        <v>158</v>
-      </c>
       <c r="C26">
         <v>1</v>
       </c>
@@ -7299,9 +7263,6 @@
       <c r="A27" t="s">
         <v>38</v>
       </c>
-      <c r="B27" t="s">
-        <v>158</v>
-      </c>
       <c r="C27">
         <v>1</v>
       </c>
@@ -7373,9 +7334,6 @@
       <c r="A28" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
-        <v>158</v>
-      </c>
       <c r="C28">
         <v>1</v>
       </c>
@@ -7447,9 +7405,6 @@
       <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B29" t="s">
-        <v>158</v>
-      </c>
       <c r="C29">
         <v>1</v>
       </c>
@@ -7518,9 +7473,6 @@
       <c r="A30" t="s">
         <v>136</v>
       </c>
-      <c r="B30" t="s">
-        <v>158</v>
-      </c>
       <c r="C30">
         <v>1</v>
       </c>
@@ -7589,9 +7541,6 @@
       <c r="A31" t="s">
         <v>72</v>
       </c>
-      <c r="B31" t="s">
-        <v>158</v>
-      </c>
       <c r="C31">
         <v>1</v>
       </c>
@@ -7660,9 +7609,6 @@
       <c r="A32" t="s">
         <v>72</v>
       </c>
-      <c r="B32" t="s">
-        <v>158</v>
-      </c>
       <c r="D32">
         <v>1</v>
       </c>
@@ -7731,9 +7677,6 @@
       <c r="A33" t="s">
         <v>137</v>
       </c>
-      <c r="B33" t="s">
-        <v>158</v>
-      </c>
       <c r="C33">
         <v>1</v>
       </c>
@@ -7802,9 +7745,6 @@
       <c r="A34" t="s">
         <v>137</v>
       </c>
-      <c r="B34" t="s">
-        <v>158</v>
-      </c>
       <c r="D34">
         <v>1</v>
       </c>
@@ -7873,9 +7813,6 @@
       <c r="A35" t="s">
         <v>138</v>
       </c>
-      <c r="B35" t="s">
-        <v>158</v>
-      </c>
       <c r="C35">
         <v>1</v>
       </c>
@@ -7947,9 +7884,6 @@
       <c r="A36" t="s">
         <v>84</v>
       </c>
-      <c r="B36" t="s">
-        <v>158</v>
-      </c>
       <c r="C36">
         <v>1</v>
       </c>
@@ -8018,9 +7952,6 @@
       <c r="A37" t="s">
         <v>76</v>
       </c>
-      <c r="B37" t="s">
-        <v>158</v>
-      </c>
       <c r="C37">
         <v>1</v>
       </c>
@@ -8092,9 +8023,6 @@
       <c r="A38" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>158</v>
-      </c>
       <c r="C38">
         <v>1</v>
       </c>
@@ -8163,9 +8091,6 @@
       <c r="A39" t="s">
         <v>109</v>
       </c>
-      <c r="B39" t="s">
-        <v>158</v>
-      </c>
       <c r="C39">
         <v>1</v>
       </c>
@@ -8234,9 +8159,6 @@
       <c r="A40" t="s">
         <v>16</v>
       </c>
-      <c r="B40" t="s">
-        <v>158</v>
-      </c>
       <c r="E40">
         <v>1</v>
       </c>
@@ -8302,9 +8224,6 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" t="s">
-        <v>158</v>
-      </c>
       <c r="E41">
         <v>1</v>
       </c>
@@ -8370,9 +8289,6 @@
       <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="B42" t="s">
-        <v>158</v>
-      </c>
       <c r="E42">
         <v>1</v>
       </c>
@@ -8438,9 +8354,6 @@
       <c r="A43" t="s">
         <v>34</v>
       </c>
-      <c r="B43" t="s">
-        <v>158</v>
-      </c>
       <c r="E43">
         <v>1</v>
       </c>
@@ -8506,9 +8419,6 @@
       <c r="A44" t="s">
         <v>8</v>
       </c>
-      <c r="B44" t="s">
-        <v>158</v>
-      </c>
       <c r="E44">
         <v>1</v>
       </c>
@@ -8574,9 +8484,6 @@
       <c r="A45" t="s">
         <v>5</v>
       </c>
-      <c r="B45" t="s">
-        <v>158</v>
-      </c>
       <c r="E45">
         <v>1</v>
       </c>
@@ -8642,9 +8549,6 @@
       <c r="A46" t="s">
         <v>13</v>
       </c>
-      <c r="B46" t="s">
-        <v>158</v>
-      </c>
       <c r="E46">
         <v>1</v>
       </c>
@@ -8710,9 +8614,6 @@
       <c r="A47" t="s">
         <v>55</v>
       </c>
-      <c r="B47" t="s">
-        <v>158</v>
-      </c>
       <c r="E47">
         <v>1</v>
       </c>
@@ -8778,9 +8679,6 @@
       <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B48" t="s">
-        <v>158</v>
-      </c>
       <c r="E48">
         <v>1</v>
       </c>
@@ -8846,9 +8744,6 @@
       <c r="A49" t="s">
         <v>59</v>
       </c>
-      <c r="B49" t="s">
-        <v>158</v>
-      </c>
       <c r="E49">
         <v>1</v>
       </c>
@@ -8914,9 +8809,6 @@
       <c r="A50" t="s">
         <v>6</v>
       </c>
-      <c r="B50" t="s">
-        <v>158</v>
-      </c>
       <c r="E50">
         <v>1</v>
       </c>
@@ -8982,9 +8874,6 @@
       <c r="A51" t="s">
         <v>9</v>
       </c>
-      <c r="B51" t="s">
-        <v>158</v>
-      </c>
       <c r="E51">
         <v>1</v>
       </c>
@@ -9050,9 +8939,6 @@
       <c r="A52" t="s">
         <v>38</v>
       </c>
-      <c r="B52" t="s">
-        <v>158</v>
-      </c>
       <c r="E52">
         <v>1</v>
       </c>
@@ -9118,9 +9004,6 @@
       <c r="A53" t="s">
         <v>20</v>
       </c>
-      <c r="B53" t="s">
-        <v>158</v>
-      </c>
       <c r="E53">
         <v>1</v>
       </c>
@@ -9186,9 +9069,6 @@
       <c r="A54" t="s">
         <v>10</v>
       </c>
-      <c r="B54" t="s">
-        <v>158</v>
-      </c>
       <c r="E54">
         <v>1</v>
       </c>
@@ -9254,9 +9134,6 @@
       <c r="A55" t="s">
         <v>136</v>
       </c>
-      <c r="B55" t="s">
-        <v>158</v>
-      </c>
       <c r="E55">
         <v>1</v>
       </c>
@@ -9322,9 +9199,6 @@
       <c r="A56" t="s">
         <v>72</v>
       </c>
-      <c r="B56" t="s">
-        <v>158</v>
-      </c>
       <c r="E56">
         <v>1</v>
       </c>
@@ -9390,9 +9264,6 @@
       <c r="A57" t="s">
         <v>137</v>
       </c>
-      <c r="B57" t="s">
-        <v>158</v>
-      </c>
       <c r="E57">
         <v>1</v>
       </c>
@@ -9458,9 +9329,6 @@
       <c r="A58" t="s">
         <v>138</v>
       </c>
-      <c r="B58" t="s">
-        <v>158</v>
-      </c>
       <c r="E58">
         <v>1</v>
       </c>
@@ -9526,9 +9394,6 @@
       <c r="A59" t="s">
         <v>84</v>
       </c>
-      <c r="B59" t="s">
-        <v>158</v>
-      </c>
       <c r="E59">
         <v>1</v>
       </c>
@@ -9594,9 +9459,6 @@
       <c r="A60" t="s">
         <v>76</v>
       </c>
-      <c r="B60" t="s">
-        <v>158</v>
-      </c>
       <c r="E60">
         <v>1</v>
       </c>
@@ -9662,9 +9524,6 @@
       <c r="A61" t="s">
         <v>80</v>
       </c>
-      <c r="B61" t="s">
-        <v>158</v>
-      </c>
       <c r="E61">
         <v>1</v>
       </c>
@@ -9730,9 +9589,6 @@
       <c r="A62" t="s">
         <v>109</v>
       </c>
-      <c r="B62" t="s">
-        <v>158</v>
-      </c>
       <c r="E62">
         <v>1</v>
       </c>
@@ -9798,9 +9654,6 @@
       <c r="A63" t="s">
         <v>4</v>
       </c>
-      <c r="B63" t="s">
-        <v>158</v>
-      </c>
       <c r="H63">
         <v>1</v>
       </c>
@@ -9866,9 +9719,6 @@
       <c r="A64" t="s">
         <v>34</v>
       </c>
-      <c r="B64" t="s">
-        <v>158</v>
-      </c>
       <c r="H64">
         <v>1</v>
       </c>
@@ -9934,9 +9784,6 @@
       <c r="A65" t="s">
         <v>13</v>
       </c>
-      <c r="B65" t="s">
-        <v>158</v>
-      </c>
       <c r="H65">
         <v>1</v>
       </c>
@@ -10002,9 +9849,6 @@
       <c r="A66" t="s">
         <v>55</v>
       </c>
-      <c r="B66" t="s">
-        <v>158</v>
-      </c>
       <c r="H66">
         <v>1</v>
       </c>
@@ -10070,9 +9914,6 @@
       <c r="A67" t="s">
         <v>52</v>
       </c>
-      <c r="B67" t="s">
-        <v>158</v>
-      </c>
       <c r="H67">
         <v>1</v>
       </c>
@@ -10138,9 +9979,6 @@
       <c r="A68" t="s">
         <v>59</v>
       </c>
-      <c r="B68" t="s">
-        <v>158</v>
-      </c>
       <c r="H68">
         <v>1</v>
       </c>
@@ -10206,9 +10044,6 @@
       <c r="A69" t="s">
         <v>38</v>
       </c>
-      <c r="B69" t="s">
-        <v>158</v>
-      </c>
       <c r="H69">
         <v>1</v>
       </c>
@@ -10274,9 +10109,6 @@
       <c r="A70" t="s">
         <v>20</v>
       </c>
-      <c r="B70" t="s">
-        <v>158</v>
-      </c>
       <c r="H70">
         <v>1</v>
       </c>
@@ -10342,9 +10174,6 @@
       <c r="A71" t="s">
         <v>138</v>
       </c>
-      <c r="B71" t="s">
-        <v>158</v>
-      </c>
       <c r="H71">
         <v>1</v>
       </c>
@@ -10410,9 +10239,6 @@
       <c r="A72" t="s">
         <v>76</v>
       </c>
-      <c r="B72" t="s">
-        <v>158</v>
-      </c>
       <c r="H72">
         <v>1</v>
       </c>
@@ -10478,9 +10304,6 @@
       <c r="A73" t="s">
         <v>80</v>
       </c>
-      <c r="B73" t="s">
-        <v>158</v>
-      </c>
       <c r="H73">
         <v>1</v>
       </c>
@@ -10545,9 +10368,6 @@
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>109</v>
-      </c>
-      <c r="B74" t="s">
-        <v>158</v>
       </c>
       <c r="H74">
         <v>1</v>

</xml_diff>